<commit_message>
Add map to dishes form using the locate app
</commit_message>
<xml_diff>
--- a/xlsforms/Dishes.xlsx
+++ b/xlsforms/Dishes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="69">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -39,88 +39,121 @@
     <t xml:space="preserve">default</t>
   </si>
   <si>
-    <t xml:space="preserve">hint</t>
+    <t xml:space="preserve">constraint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dish_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of dish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">begin repeat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ingredients</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingredients</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wq:initial(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one ingredient_choices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ingredient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingredient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">decimal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity (in gramms)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one origin_choices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">origin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Place of origin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end repeat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">photos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photos</t>
   </si>
   <si>
     <t xml:space="preserve">image</t>
   </si>
   <si>
-    <t xml:space="preserve">constraint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">appearance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dish_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name of dish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">begin repeat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ingredients</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ingredients</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one ingredients_choices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ingredient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ingredient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">decimal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">quantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantity (in gramms)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one origin_choices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">origin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Place of origin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end repeat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">photos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Photos</t>
-  </si>
-  <si>
     <t xml:space="preserve">photo</t>
   </si>
   <si>
     <t xml:space="preserve">Photo</t>
   </si>
   <si>
+    <t xml:space="preserve">select_one location_choices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location Mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geopoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geometry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accuracy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPS Accuracy</t>
+  </si>
+  <si>
     <t xml:space="preserve">list name</t>
   </si>
   <si>
-    <t xml:space="preserve">ingredients_choices</t>
+    <t xml:space="preserve">ingredient_choices</t>
   </si>
   <si>
     <t xml:space="preserve">potatoes</t>
@@ -135,10 +168,10 @@
     <t xml:space="preserve">Cucumber</t>
   </si>
   <si>
-    <t xml:space="preserve">meat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Meat</t>
+    <t xml:space="preserve">chicken_meat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chicken meat</t>
   </si>
   <si>
     <t xml:space="preserve">origin_choices</t>
@@ -154,6 +187,27 @@
   </si>
   <si>
     <t xml:space="preserve">Non-local</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location_choices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use GPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interactive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Point on Map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter Manually</t>
   </si>
   <si>
     <t xml:space="preserve">form_title</t>
@@ -184,7 +238,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -247,6 +301,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
@@ -307,7 +367,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -316,7 +376,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -360,7 +420,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -443,16 +507,18 @@
   </sheetPr>
   <dimension ref="A1:AMJ34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="31.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="1" width="31.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="31.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="31.28"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="5" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -468,141 +534,219 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="0"/>
+      <c r="I1" s="4"/>
       <c r="AMI1" s="1"/>
       <c r="AMJ1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" s="6" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C4" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" s="6" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="7" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+      <c r="C5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="9"/>
-    </row>
-    <row r="6" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+      <c r="C6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="B7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="9"/>
-    </row>
-    <row r="7" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+      <c r="C7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" s="6" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" s="6" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" s="6" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" s="6" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="B14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="0"/>
+    </row>
+    <row r="19" s="6" customFormat="true" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H19" s="0"/>
+    </row>
     <row r="20" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -668,10 +812,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -685,7 +829,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>1</v>
@@ -696,62 +840,95 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="0"/>
+    </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -796,33 +973,33 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="13" t="n">
+      <c r="A2" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="13"/>
+      <c r="E2" s="14"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>